<commit_message>
premier jet cross validation rapport finale
</commit_message>
<xml_diff>
--- a/Remise/Remise 4/matrice_verification.xlsx
+++ b/Remise/Remise 4/matrice_verification.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="40" windowWidth="23720" windowHeight="10040"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="23715" windowHeight="10035"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -155,9 +155,6 @@
     <t>Oui</t>
   </si>
   <si>
-    <t>t=0.31s, Pmoy = 2.53MW et Pmax=3.55MW pour PSIM, Pmoy=2.58MW et Pmax=3.56MW pour SPS</t>
-  </si>
-  <si>
     <t>±15A</t>
   </si>
   <si>
@@ -186,6 +183,9 @@
   </si>
   <si>
     <t>Temps de recharge  de 0.31s calculé à partir du point bas de la tension du bus CC (variation de 1700V)</t>
+  </si>
+  <si>
+    <t>t=0.31s, Pmoy = 2.53MW et Pmax=3.6MW pour PSIM, Pmoy=2.58MW et Pmax=3.56MW pour SPS</t>
   </si>
 </sst>
 </file>
@@ -396,6 +396,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -408,20 +414,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Lien hypertexte visité" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -721,25 +721,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
-    <col min="4" max="4" width="36.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="6" max="6" width="22.6640625" customWidth="1"/>
-    <col min="7" max="7" width="14.1640625" customWidth="1"/>
-    <col min="8" max="8" width="37.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="36.85546875" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="8" max="8" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -765,8 +768,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -782,17 +785,17 @@
         <v>15</v>
       </c>
       <c r="F2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1">
-      <c r="A3" s="10"/>
+    </row>
+    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="12"/>
       <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
@@ -804,15 +807,15 @@
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="63" customHeight="1">
-      <c r="A4" s="11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -828,15 +831,15 @@
         <v>15</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="14" t="s">
         <v>45</v>
       </c>
+      <c r="G4" s="10" t="s">
+        <v>44</v>
+      </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" ht="60">
-      <c r="A5" s="11"/>
+    <row r="5" spans="1:8" ht="87.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
       <c r="B5" s="2" t="s">
         <v>19</v>
       </c>
@@ -850,15 +853,15 @@
         <v>15</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="15" t="s">
-        <v>46</v>
-      </c>
       <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8" ht="30">
-      <c r="A6" s="12"/>
+    <row r="6" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="14"/>
       <c r="B6" s="2" t="s">
         <v>22</v>
       </c>
@@ -875,8 +878,8 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="63" customHeight="1">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -889,20 +892,20 @@
         <v>28</v>
       </c>
       <c r="E7" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="H7" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="60">
-      <c r="A8" s="12"/>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="14"/>
       <c r="B8" s="2" t="s">
         <v>29</v>
       </c>
@@ -916,15 +919,15 @@
         <v>31</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>53</v>
-      </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="30">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>32</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -943,8 +946,8 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="45">
-      <c r="A10" s="12"/>
+    <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="14"/>
       <c r="B10" s="2" t="s">
         <v>36</v>
       </c>
@@ -961,8 +964,8 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" ht="45">
-      <c r="A11" s="13" t="s">
+    <row r="11" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -981,8 +984,8 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="30">
-      <c r="A12" s="11"/>
+    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="13"/>
       <c r="B12" s="2" t="s">
         <v>40</v>
       </c>
@@ -999,8 +1002,8 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" ht="45">
-      <c r="A13" s="12"/>
+    <row r="13" spans="1:8" ht="63" x14ac:dyDescent="0.25">
+      <c r="A13" s="14"/>
       <c r="B13" s="2" t="s">
         <v>41</v>
       </c>
@@ -1025,8 +1028,8 @@
     <mergeCell ref="A9:A10"/>
     <mergeCell ref="A11:A13"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1041,7 +1044,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1058,7 +1061,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Ajout d'images dans le rapport final
</commit_message>
<xml_diff>
--- a/Remise/Remise 4/matrice_verification.xlsx
+++ b/Remise/Remise 4/matrice_verification.xlsx
@@ -173,9 +173,6 @@
     <t>t≤2s, Pmax≤3.6MW, Pmoy ≤2.7MW</t>
   </si>
   <si>
-    <t xml:space="preserve">Δt = 1.69s, ΔPmoy = -0.17MW, ΔPmax = -0.04MW </t>
-  </si>
-  <si>
     <t>ΔVmax = 0.2, Δφ = 0.3</t>
   </si>
   <si>
@@ -185,7 +182,10 @@
     <t>Temps de recharge  de 0.31s calculé à partir du point bas de la tension du bus CC (variation de 1700V)</t>
   </si>
   <si>
-    <t>t=0.31s, Pmoy = 2.53MW et Pmax=3.6MW pour PSIM, Pmoy=2.58MW et Pmax=3.56MW pour SPS</t>
+    <t xml:space="preserve">Δt = 1.69s, ΔPmoy = -0.15MW, ΔPmax = -0.04MW </t>
+  </si>
+  <si>
+    <t>t=0.31s, Pmoy = 2.55MW et Pmax=3.62MW pour PSIM, Pmoy=2.48MW et Pmax=3.56MW pour SPS</t>
   </si>
 </sst>
 </file>
@@ -726,8 +726,8 @@
   </sheetPr>
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -768,7 +768,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>8</v>
       </c>
@@ -794,7 +794,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="12"/>
       <c r="B3" s="4" t="s">
         <v>10</v>
@@ -878,7 +878,7 @@
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
     </row>
-    <row r="7" spans="1:8" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>25</v>
       </c>
@@ -898,13 +898,13 @@
         <v>54</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="14"/>
       <c r="B8" s="2" t="s">
         <v>29</v>
@@ -919,14 +919,14 @@
         <v>31</v>
       </c>
       <c r="F8" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="G8" s="4" t="s">
-        <v>52</v>
-      </c>
       <c r="H8" s="4"/>
     </row>
-    <row r="9" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>32</v>
       </c>
@@ -946,7 +946,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="2" t="s">
         <v>36</v>
@@ -984,7 +984,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="2" t="s">
         <v>40</v>

</xml_diff>